<commit_message>
Listados casi listos del 30 de agosto
</commit_message>
<xml_diff>
--- a/Agosto/30 agosto/costa chica/LISTA DE ALUMNOS PARA ENVIO EVALUATEC 2DA APPLICACION ENVIO 23 de agosto (1).xlsx
+++ b/Agosto/30 agosto/costa chica/LISTA DE ALUMNOS PARA ENVIO EVALUATEC 2DA APPLICACION ENVIO 23 de agosto (1).xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28020"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_D61BFC23C1589F265F97B2DF47148AB80ADC06EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Proyecto01TICs\Documents\Evaluatec2024\Agosto\30 agosto\costa chica\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB4D7EB-DE0C-4537-8BB1-2398E3865729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ING.CIVIL" sheetId="3" r:id="rId1"/>
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="406">
   <si>
     <t>INDICAR SI EL ASPIRANTE DEBE PRESENTARSE EN EL PLANTEL PARA REALIZAR EL EXAMEN</t>
   </si>
@@ -1257,7 +1262,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1387,98 +1392,138 @@
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="38">
     <dxf>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="h:mm\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="h:mm\ AM/PM"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <numFmt numFmtId="165" formatCode="h:mm\ AM/PM"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <numFmt numFmtId="165" formatCode="h:mm\ AM/PM"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <numFmt numFmtId="165" formatCode="h:mm\ AM/PM"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <numFmt numFmtId="165" formatCode="h:mm\ AM/PM"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <numFmt numFmtId="165" formatCode="h:mm\ AM/PM"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <numFmt numFmtId="165" formatCode="h:mm\ AM/PM"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <numFmt numFmtId="165" formatCode="h:mm\ AM/PM"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <numFmt numFmtId="165" formatCode="h:mm\ AM/PM"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <numFmt numFmtId="165" formatCode="h:mm\ AM/PM"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <numFmt numFmtId="165" formatCode="h:mm\ AM/PM"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <numFmt numFmtId="165" formatCode="h:mm\ AM/PM"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <numFmt numFmtId="165" formatCode="h:mm\ AM/PM"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <numFmt numFmtId="165" formatCode="h:mm\ AM/PM"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <numFmt numFmtId="165" formatCode="h:mm\ AM/PM"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <numFmt numFmtId="165" formatCode="h:mm\ AM/PM"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <numFmt numFmtId="165" formatCode="h:mm\ AM/PM"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <numFmt numFmtId="165" formatCode="h:mm\ AM/PM"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <numFmt numFmtId="165" formatCode="h:mm\ AM/PM"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
@@ -1547,20 +1592,20 @@
     <sortCondition ref="C5:C107"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="FICHA" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NOMBRE ASPIRANTE" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="CURP" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="CORREO ELECTRONICO" dataDxfId="30" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="FICHA" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NOMBRE ASPIRANTE" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="CURP" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="CORREO ELECTRONICO" dataDxfId="34" dataCellStyle="Hipervínculo"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="CLAVE DE CARRERA"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="CLAVE CARRERA" dataCellStyle="Hipervínculo"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="CARRERA"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="VERSION"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="FECHA SIMULACRO" dataDxfId="29"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="HORA DE SIMULACRO" dataDxfId="28"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="FECHA APLICACIÓN OFICIAL" dataDxfId="27"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="HORA APLICACIÓN OFICIAL" dataDxfId="26"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="¿ASPIRANTE EN PLANTEL?" dataDxfId="25"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="AULA" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="FECHA SIMULACRO" dataDxfId="33"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="HORA DE SIMULACRO" dataDxfId="32"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="FECHA APLICACIÓN OFICIAL" dataDxfId="31"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="HORA APLICACIÓN OFICIAL" dataDxfId="30"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="¿ASPIRANTE EN PLANTEL?" dataDxfId="29"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="AULA" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1580,22 +1625,22 @@
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="CLAVE CARRERA" dataCellStyle="Hipervínculo"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="CARRERA"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="VERSION"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="FECHA SIMULACRO" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="HORA DE SIMULACRO" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="FECHA APLICACIÓN OFICIAL" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="HORA APLICACIÓN OFICIAL" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="¿ASPIRANTE EN PLANTEL?" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="AULA" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="FECHA SIMULACRO" dataDxfId="27"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="HORA DE SIMULACRO" dataDxfId="26"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="FECHA APLICACIÓN OFICIAL" dataDxfId="25"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="HORA APLICACIÓN OFICIAL" dataDxfId="24"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="¿ASPIRANTE EN PLANTEL?" dataDxfId="23"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="AULA" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabla22456" displayName="Tabla22456" ref="B4:N56" totalsRowShown="0">
-  <autoFilter ref="B4:N56" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:N56">
-    <sortCondition ref="C5:C56"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabla22456" displayName="Tabla22456" ref="B4:N55" totalsRowShown="0">
+  <autoFilter ref="B4:N55" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:N55">
+    <sortCondition ref="C5:C55"/>
   </sortState>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="FICHA"/>
@@ -1605,12 +1650,12 @@
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="CLAVE CARRERA" dataCellStyle="Hipervínculo"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="CARRERA"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="VERSION"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="FECHA SIMULACRO" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="HORA DE SIMULACRO" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="FECHA APLICACIÓN OFICIAL" dataDxfId="15"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="HORA APLICACIÓN OFICIAL" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="¿ASPIRANTE EN PLANTEL?" dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="AULA" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="FECHA SIMULACRO" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="HORA DE SIMULACRO" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="FECHA APLICACIÓN OFICIAL" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="HORA APLICACIÓN OFICIAL" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="¿ASPIRANTE EN PLANTEL?" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="AULA" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1630,12 +1675,12 @@
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0300-00000D000000}" name="CLAVE CARRERA" dataCellStyle="Hipervínculo"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="CARRERA"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="VERSION"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="FECHA SIMULACRO" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="HORA DE SIMULACRO" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="FECHA APLICACIÓN OFICIAL" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="HORA APLICACIÓN OFICIAL" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="¿ASPIRANTE EN PLANTEL?" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0300-00000C000000}" name="AULA" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="FECHA SIMULACRO" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="HORA DE SIMULACRO" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="FECHA APLICACIÓN OFICIAL" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="HORA APLICACIÓN OFICIAL" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="¿ASPIRANTE EN PLANTEL?" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0300-00000C000000}" name="AULA" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1655,12 +1700,12 @@
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0400-00000D000000}" name="CLAVE CARRERA" dataCellStyle="Hipervínculo"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="CARRERA"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="VERSION"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="FECHA SIMULACRO" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="HORA DE SIMULACRO" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="FECHA APLICACIÓN OFICIAL" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="HORA APLICACIÓN OFICIAL" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0400-00000B000000}" name="¿ASPIRANTE EN PLANTEL?" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0400-00000C000000}" name="AULA" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="FECHA SIMULACRO" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="HORA DE SIMULACRO" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="FECHA APLICACIÓN OFICIAL" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="HORA APLICACIÓN OFICIAL" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0400-00000B000000}" name="¿ASPIRANTE EN PLANTEL?" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0400-00000C000000}" name="AULA" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1965,11 +2010,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O107"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34:J40"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5" style="7" customWidth="1"/>
     <col min="2" max="2" width="6.375" customWidth="1"/>
@@ -1987,12 +2032,12 @@
     <col min="15" max="15" width="8.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="41.1" customHeight="1">
+    <row r="1" spans="1:15" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N1" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="21" customHeight="1">
+    <row r="2" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
@@ -2009,13 +2054,13 @@
       <c r="L2" s="12"/>
       <c r="N2" s="11"/>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
       <c r="N3" s="11"/>
     </row>
-    <row r="4" spans="1:15" ht="31.5">
+    <row r="4" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -2059,7 +2104,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2319</v>
       </c>
@@ -2103,7 +2148,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>2318</v>
       </c>
@@ -2147,7 +2192,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>2316</v>
       </c>
@@ -2191,7 +2236,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>2315</v>
       </c>
@@ -2235,7 +2280,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>2313</v>
       </c>
@@ -2279,7 +2324,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>2291</v>
       </c>
@@ -2323,7 +2368,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>2268</v>
       </c>
@@ -2367,7 +2412,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>2248</v>
       </c>
@@ -2411,7 +2456,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>2239</v>
       </c>
@@ -2455,7 +2500,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>2230</v>
       </c>
@@ -2499,7 +2544,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>2220</v>
       </c>
@@ -2543,7 +2588,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>2219</v>
       </c>
@@ -2587,7 +2632,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="2:15">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>2217</v>
       </c>
@@ -2631,7 +2676,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:15">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>2213</v>
       </c>
@@ -2675,7 +2720,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:15">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>2209</v>
       </c>
@@ -2719,7 +2764,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="2:15">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>2206</v>
       </c>
@@ -2763,7 +2808,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="2:15">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>2199</v>
       </c>
@@ -2807,7 +2852,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="2:15">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>2192</v>
       </c>
@@ -2851,7 +2896,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="2:15">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>1738</v>
       </c>
@@ -2895,7 +2940,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="2:15">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>1835</v>
       </c>
@@ -2939,7 +2984,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="2:15">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>2361</v>
       </c>
@@ -2983,7 +3028,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="2:15">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>2350</v>
       </c>
@@ -3027,7 +3072,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="2:15">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>2338</v>
       </c>
@@ -3071,7 +3116,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="2:15">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>2334</v>
       </c>
@@ -3115,7 +3160,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="2:15">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>2331</v>
       </c>
@@ -3159,7 +3204,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="2:15">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>2372</v>
       </c>
@@ -3203,7 +3248,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="2:15">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>2367</v>
       </c>
@@ -3247,7 +3292,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="2:15">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>2366</v>
       </c>
@@ -3291,7 +3336,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="2:15">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>2362</v>
       </c>
@@ -3335,7 +3380,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="2:15">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>2374</v>
       </c>
@@ -3379,7 +3424,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="2:15">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>2398</v>
       </c>
@@ -3423,7 +3468,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="2:15">
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>2386</v>
       </c>
@@ -3467,7 +3512,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="2:15">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>2385</v>
       </c>
@@ -3511,7 +3556,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="2:15">
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>2409</v>
       </c>
@@ -3555,7 +3600,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="2:15">
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>2422</v>
       </c>
@@ -3597,7 +3642,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="2:15">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>2421</v>
       </c>
@@ -3641,7 +3686,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="2:15">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
@@ -3654,7 +3699,7 @@
       <c r="N41" s="6"/>
       <c r="O41" s="5"/>
     </row>
-    <row r="42" spans="2:15">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
@@ -3667,7 +3712,7 @@
       <c r="N42" s="6"/>
       <c r="O42" s="5"/>
     </row>
-    <row r="43" spans="2:15">
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
@@ -3680,7 +3725,7 @@
       <c r="N43" s="6"/>
       <c r="O43" s="5"/>
     </row>
-    <row r="44" spans="2:15">
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
@@ -3693,7 +3738,7 @@
       <c r="N44" s="6"/>
       <c r="O44" s="5"/>
     </row>
-    <row r="45" spans="2:15">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
@@ -3706,7 +3751,7 @@
       <c r="N45" s="6"/>
       <c r="O45" s="5"/>
     </row>
-    <row r="46" spans="2:15">
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
@@ -3719,7 +3764,7 @@
       <c r="N46" s="6"/>
       <c r="O46" s="5"/>
     </row>
-    <row r="47" spans="2:15">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
@@ -3733,7 +3778,7 @@
       <c r="N47" s="6"/>
       <c r="O47" s="5"/>
     </row>
-    <row r="48" spans="2:15">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
@@ -3746,7 +3791,7 @@
       <c r="N48" s="6"/>
       <c r="O48" s="5"/>
     </row>
-    <row r="49" spans="2:15">
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
@@ -3759,7 +3804,7 @@
       <c r="N49" s="6"/>
       <c r="O49" s="5"/>
     </row>
-    <row r="50" spans="2:15">
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
@@ -3772,7 +3817,7 @@
       <c r="N50" s="6"/>
       <c r="O50" s="5"/>
     </row>
-    <row r="51" spans="2:15">
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
@@ -3785,7 +3830,7 @@
       <c r="N51" s="6"/>
       <c r="O51" s="5"/>
     </row>
-    <row r="52" spans="2:15">
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
@@ -3798,7 +3843,7 @@
       <c r="N52" s="6"/>
       <c r="O52" s="5"/>
     </row>
-    <row r="53" spans="2:15">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
@@ -3811,7 +3856,7 @@
       <c r="N53" s="6"/>
       <c r="O53" s="5"/>
     </row>
-    <row r="54" spans="2:15">
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
@@ -3824,7 +3869,7 @@
       <c r="N54" s="6"/>
       <c r="O54" s="5"/>
     </row>
-    <row r="55" spans="2:15">
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
@@ -3837,7 +3882,7 @@
       <c r="N55" s="6"/>
       <c r="O55" s="5"/>
     </row>
-    <row r="56" spans="2:15">
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
@@ -3850,7 +3895,7 @@
       <c r="N56" s="6"/>
       <c r="O56" s="5"/>
     </row>
-    <row r="57" spans="2:15">
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
@@ -3863,7 +3908,7 @@
       <c r="N57" s="6"/>
       <c r="O57" s="5"/>
     </row>
-    <row r="58" spans="2:15">
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
@@ -3876,7 +3921,7 @@
       <c r="N58" s="6"/>
       <c r="O58" s="5"/>
     </row>
-    <row r="59" spans="2:15">
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
@@ -3889,7 +3934,7 @@
       <c r="N59" s="6"/>
       <c r="O59" s="5"/>
     </row>
-    <row r="60" spans="2:15">
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
@@ -3902,7 +3947,7 @@
       <c r="N60" s="6"/>
       <c r="O60" s="5"/>
     </row>
-    <row r="61" spans="2:15">
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
@@ -3915,7 +3960,7 @@
       <c r="N61" s="6"/>
       <c r="O61" s="5"/>
     </row>
-    <row r="62" spans="2:15">
+    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
@@ -3928,7 +3973,7 @@
       <c r="N62" s="6"/>
       <c r="O62" s="5"/>
     </row>
-    <row r="63" spans="2:15">
+    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
@@ -3941,7 +3986,7 @@
       <c r="N63" s="6"/>
       <c r="O63" s="5"/>
     </row>
-    <row r="64" spans="2:15">
+    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
@@ -3954,7 +3999,7 @@
       <c r="N64" s="6"/>
       <c r="O64" s="5"/>
     </row>
-    <row r="65" spans="2:15">
+    <row r="65" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
@@ -3967,7 +4012,7 @@
       <c r="N65" s="6"/>
       <c r="O65" s="5"/>
     </row>
-    <row r="66" spans="2:15">
+    <row r="66" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
@@ -3980,7 +4025,7 @@
       <c r="N66" s="6"/>
       <c r="O66" s="5"/>
     </row>
-    <row r="67" spans="2:15">
+    <row r="67" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
@@ -3993,7 +4038,7 @@
       <c r="N67" s="6"/>
       <c r="O67" s="5"/>
     </row>
-    <row r="68" spans="2:15">
+    <row r="68" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
@@ -4006,7 +4051,7 @@
       <c r="N68" s="6"/>
       <c r="O68" s="5"/>
     </row>
-    <row r="69" spans="2:15">
+    <row r="69" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
@@ -4019,7 +4064,7 @@
       <c r="N69" s="6"/>
       <c r="O69" s="5"/>
     </row>
-    <row r="70" spans="2:15">
+    <row r="70" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
@@ -4032,7 +4077,7 @@
       <c r="N70" s="6"/>
       <c r="O70" s="5"/>
     </row>
-    <row r="71" spans="2:15">
+    <row r="71" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
@@ -4045,7 +4090,7 @@
       <c r="N71" s="6"/>
       <c r="O71" s="5"/>
     </row>
-    <row r="72" spans="2:15">
+    <row r="72" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
@@ -4058,7 +4103,7 @@
       <c r="N72" s="6"/>
       <c r="O72" s="5"/>
     </row>
-    <row r="73" spans="2:15">
+    <row r="73" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
@@ -4071,7 +4116,7 @@
       <c r="N73" s="6"/>
       <c r="O73" s="5"/>
     </row>
-    <row r="74" spans="2:15">
+    <row r="74" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
@@ -4084,7 +4129,7 @@
       <c r="N74" s="6"/>
       <c r="O74" s="5"/>
     </row>
-    <row r="75" spans="2:15">
+    <row r="75" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
@@ -4097,7 +4142,7 @@
       <c r="N75" s="6"/>
       <c r="O75" s="5"/>
     </row>
-    <row r="76" spans="2:15">
+    <row r="76" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
@@ -4110,7 +4155,7 @@
       <c r="N76" s="6"/>
       <c r="O76" s="5"/>
     </row>
-    <row r="77" spans="2:15">
+    <row r="77" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
@@ -4124,7 +4169,7 @@
       <c r="N77" s="6"/>
       <c r="O77" s="5"/>
     </row>
-    <row r="78" spans="2:15">
+    <row r="78" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
@@ -4137,7 +4182,7 @@
       <c r="N78" s="6"/>
       <c r="O78" s="5"/>
     </row>
-    <row r="79" spans="2:15">
+    <row r="79" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
@@ -4150,7 +4195,7 @@
       <c r="N79" s="6"/>
       <c r="O79" s="5"/>
     </row>
-    <row r="80" spans="2:15">
+    <row r="80" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
@@ -4163,7 +4208,7 @@
       <c r="N80" s="6"/>
       <c r="O80" s="5"/>
     </row>
-    <row r="81" spans="2:15">
+    <row r="81" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
@@ -4176,7 +4221,7 @@
       <c r="N81" s="6"/>
       <c r="O81" s="5"/>
     </row>
-    <row r="82" spans="2:15">
+    <row r="82" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
       <c r="D82" s="7"/>
@@ -4189,7 +4234,7 @@
       <c r="N82" s="6"/>
       <c r="O82" s="5"/>
     </row>
-    <row r="83" spans="2:15">
+    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
       <c r="D83" s="7"/>
@@ -4202,7 +4247,7 @@
       <c r="N83" s="6"/>
       <c r="O83" s="5"/>
     </row>
-    <row r="84" spans="2:15">
+    <row r="84" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
       <c r="D84" s="7"/>
@@ -4216,7 +4261,7 @@
       <c r="N84" s="6"/>
       <c r="O84" s="5"/>
     </row>
-    <row r="85" spans="2:15">
+    <row r="85" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
@@ -4229,7 +4274,7 @@
       <c r="N85" s="6"/>
       <c r="O85" s="5"/>
     </row>
-    <row r="86" spans="2:15">
+    <row r="86" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
@@ -4242,7 +4287,7 @@
       <c r="N86" s="6"/>
       <c r="O86" s="5"/>
     </row>
-    <row r="87" spans="2:15">
+    <row r="87" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
       <c r="D87" s="7"/>
@@ -4255,7 +4300,7 @@
       <c r="N87" s="6"/>
       <c r="O87" s="5"/>
     </row>
-    <row r="88" spans="2:15">
+    <row r="88" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
@@ -4268,7 +4313,7 @@
       <c r="N88" s="6"/>
       <c r="O88" s="5"/>
     </row>
-    <row r="89" spans="2:15">
+    <row r="89" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
       <c r="D89" s="7"/>
@@ -4281,7 +4326,7 @@
       <c r="N89" s="6"/>
       <c r="O89" s="5"/>
     </row>
-    <row r="90" spans="2:15">
+    <row r="90" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
@@ -4294,7 +4339,7 @@
       <c r="N90" s="6"/>
       <c r="O90" s="5"/>
     </row>
-    <row r="91" spans="2:15">
+    <row r="91" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
       <c r="D91" s="7"/>
@@ -4307,7 +4352,7 @@
       <c r="N91" s="6"/>
       <c r="O91" s="5"/>
     </row>
-    <row r="92" spans="2:15">
+    <row r="92" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
       <c r="D92" s="7"/>
@@ -4320,7 +4365,7 @@
       <c r="N92" s="6"/>
       <c r="O92" s="5"/>
     </row>
-    <row r="93" spans="2:15">
+    <row r="93" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
       <c r="D93" s="7"/>
@@ -4333,7 +4378,7 @@
       <c r="N93" s="6"/>
       <c r="O93" s="5"/>
     </row>
-    <row r="94" spans="2:15">
+    <row r="94" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
       <c r="D94" s="7"/>
@@ -4346,7 +4391,7 @@
       <c r="N94" s="6"/>
       <c r="O94" s="5"/>
     </row>
-    <row r="95" spans="2:15">
+    <row r="95" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
       <c r="D95" s="7"/>
@@ -4359,7 +4404,7 @@
       <c r="N95" s="6"/>
       <c r="O95" s="5"/>
     </row>
-    <row r="96" spans="2:15">
+    <row r="96" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
       <c r="D96" s="7"/>
@@ -4372,7 +4417,7 @@
       <c r="N96" s="6"/>
       <c r="O96" s="5"/>
     </row>
-    <row r="97" spans="2:15">
+    <row r="97" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
       <c r="D97" s="7"/>
@@ -4385,7 +4430,7 @@
       <c r="N97" s="6"/>
       <c r="O97" s="5"/>
     </row>
-    <row r="98" spans="2:15">
+    <row r="98" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
       <c r="D98" s="7"/>
@@ -4398,7 +4443,7 @@
       <c r="N98" s="6"/>
       <c r="O98" s="5"/>
     </row>
-    <row r="99" spans="2:15">
+    <row r="99" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
       <c r="D99" s="7"/>
@@ -4411,7 +4456,7 @@
       <c r="N99" s="6"/>
       <c r="O99" s="5"/>
     </row>
-    <row r="100" spans="2:15">
+    <row r="100" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
       <c r="D100" s="7"/>
@@ -4424,7 +4469,7 @@
       <c r="N100" s="6"/>
       <c r="O100" s="5"/>
     </row>
-    <row r="101" spans="2:15">
+    <row r="101" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
       <c r="D101" s="7"/>
@@ -4437,7 +4482,7 @@
       <c r="N101" s="6"/>
       <c r="O101" s="5"/>
     </row>
-    <row r="102" spans="2:15">
+    <row r="102" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
       <c r="D102" s="7"/>
@@ -4450,7 +4495,7 @@
       <c r="N102" s="6"/>
       <c r="O102" s="5"/>
     </row>
-    <row r="103" spans="2:15">
+    <row r="103" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
       <c r="D103" s="7"/>
@@ -4463,7 +4508,7 @@
       <c r="N103" s="6"/>
       <c r="O103" s="5"/>
     </row>
-    <row r="104" spans="2:15">
+    <row r="104" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
       <c r="D104" s="7"/>
@@ -4476,7 +4521,7 @@
       <c r="N104" s="6"/>
       <c r="O104" s="5"/>
     </row>
-    <row r="105" spans="2:15">
+    <row r="105" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
       <c r="D105" s="7"/>
@@ -4489,7 +4534,7 @@
       <c r="N105" s="6"/>
       <c r="O105" s="5"/>
     </row>
-    <row r="106" spans="2:15">
+    <row r="106" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
@@ -4502,7 +4547,7 @@
       <c r="N106" s="6"/>
       <c r="O106" s="5"/>
     </row>
-    <row r="107" spans="2:15">
+    <row r="107" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
@@ -4521,6 +4566,9 @@
     <mergeCell ref="A2:L2"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="E40" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
@@ -4537,10 +4585,10 @@
   <dimension ref="B1:N45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="B5" sqref="B5:B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="8.5" customWidth="1"/>
     <col min="3" max="3" width="34.5" customWidth="1"/>
@@ -4556,12 +4604,12 @@
     <col min="14" max="14" width="8.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="41.1" customHeight="1">
+    <row r="1" spans="2:14" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M1" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:14" ht="21" customHeight="1" thickBot="1">
+    <row r="2" spans="2:14" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D2" s="13" t="s">
         <v>1</v>
       </c>
@@ -4574,10 +4622,10 @@
       <c r="K2" s="13"/>
       <c r="M2" s="11"/>
     </row>
-    <row r="3" spans="2:14" ht="16.5" thickTop="1">
+    <row r="3" spans="2:14" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="M3" s="11"/>
     </row>
-    <row r="4" spans="2:14" ht="31.5">
+    <row r="4" spans="2:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -4618,7 +4666,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:14">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2297</v>
       </c>
@@ -4659,7 +4707,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="2:14">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>2294</v>
       </c>
@@ -4700,7 +4748,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:14">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>2279</v>
       </c>
@@ -4741,7 +4789,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="2:14">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>2277</v>
       </c>
@@ -4782,7 +4830,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:14">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>2257</v>
       </c>
@@ -4823,7 +4871,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="2:14">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>2249</v>
       </c>
@@ -4864,7 +4912,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:14">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>2225</v>
       </c>
@@ -4905,7 +4953,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:14">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>2204</v>
       </c>
@@ -4946,7 +4994,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="2:14">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>2202</v>
       </c>
@@ -4987,7 +5035,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:14">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>1814</v>
       </c>
@@ -5028,7 +5076,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:14">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>2355</v>
       </c>
@@ -5069,7 +5117,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="2:14">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>2348</v>
       </c>
@@ -5110,7 +5158,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="2:14">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>2375</v>
       </c>
@@ -5151,7 +5199,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:14">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>2378</v>
       </c>
@@ -5192,7 +5240,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:14">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F19" s="1"/>
       <c r="I19" s="4"/>
       <c r="J19" s="5"/>
@@ -5201,7 +5249,7 @@
       <c r="M19" s="6"/>
       <c r="N19" s="5"/>
     </row>
-    <row r="20" spans="2:14">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F20" s="1"/>
       <c r="I20" s="4"/>
       <c r="J20" s="5"/>
@@ -5210,7 +5258,7 @@
       <c r="M20" s="6"/>
       <c r="N20" s="5"/>
     </row>
-    <row r="21" spans="2:14">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F21" s="1"/>
       <c r="I21" s="4"/>
       <c r="J21" s="5"/>
@@ -5219,7 +5267,7 @@
       <c r="M21" s="6"/>
       <c r="N21" s="5"/>
     </row>
-    <row r="22" spans="2:14">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F22" s="1"/>
       <c r="I22" s="4"/>
       <c r="J22" s="5"/>
@@ -5228,7 +5276,7 @@
       <c r="M22" s="6"/>
       <c r="N22" s="5"/>
     </row>
-    <row r="23" spans="2:14">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F23" s="1"/>
       <c r="I23" s="4"/>
       <c r="J23" s="5"/>
@@ -5237,7 +5285,7 @@
       <c r="M23" s="6"/>
       <c r="N23" s="5"/>
     </row>
-    <row r="24" spans="2:14">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F24" s="1"/>
       <c r="I24" s="4"/>
       <c r="J24" s="5"/>
@@ -5246,7 +5294,7 @@
       <c r="M24" s="6"/>
       <c r="N24" s="5"/>
     </row>
-    <row r="25" spans="2:14">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="I25" s="4"/>
@@ -5256,7 +5304,7 @@
       <c r="M25" s="6"/>
       <c r="N25" s="5"/>
     </row>
-    <row r="26" spans="2:14">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F26" s="1"/>
       <c r="I26" s="4"/>
       <c r="J26" s="5"/>
@@ -5265,7 +5313,7 @@
       <c r="M26" s="6"/>
       <c r="N26" s="5"/>
     </row>
-    <row r="27" spans="2:14">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F27" s="1"/>
       <c r="I27" s="4"/>
       <c r="J27" s="5"/>
@@ -5274,7 +5322,7 @@
       <c r="M27" s="6"/>
       <c r="N27" s="5"/>
     </row>
-    <row r="28" spans="2:14">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F28" s="1"/>
       <c r="I28" s="4"/>
       <c r="J28" s="5"/>
@@ -5283,7 +5331,7 @@
       <c r="M28" s="6"/>
       <c r="N28" s="5"/>
     </row>
-    <row r="29" spans="2:14">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F29" s="1"/>
       <c r="I29" s="4"/>
       <c r="J29" s="5"/>
@@ -5292,7 +5340,7 @@
       <c r="M29" s="6"/>
       <c r="N29" s="5"/>
     </row>
-    <row r="30" spans="2:14">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F30" s="1"/>
       <c r="I30" s="4"/>
       <c r="J30" s="5"/>
@@ -5301,7 +5349,7 @@
       <c r="M30" s="6"/>
       <c r="N30" s="5"/>
     </row>
-    <row r="31" spans="2:14">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F31" s="1"/>
       <c r="I31" s="4"/>
       <c r="J31" s="5"/>
@@ -5310,7 +5358,7 @@
       <c r="M31" s="6"/>
       <c r="N31" s="5"/>
     </row>
-    <row r="32" spans="2:14">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F32" s="1"/>
       <c r="I32" s="4"/>
       <c r="J32" s="5"/>
@@ -5319,7 +5367,7 @@
       <c r="M32" s="6"/>
       <c r="N32" s="5"/>
     </row>
-    <row r="33" spans="6:14">
+    <row r="33" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F33" s="1"/>
       <c r="I33" s="4"/>
       <c r="J33" s="5"/>
@@ -5328,7 +5376,7 @@
       <c r="M33" s="6"/>
       <c r="N33" s="5"/>
     </row>
-    <row r="34" spans="6:14">
+    <row r="34" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F34" s="1"/>
       <c r="I34" s="4"/>
       <c r="J34" s="5"/>
@@ -5337,7 +5385,7 @@
       <c r="M34" s="6"/>
       <c r="N34" s="5"/>
     </row>
-    <row r="35" spans="6:14">
+    <row r="35" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F35" s="1"/>
       <c r="I35" s="4"/>
       <c r="J35" s="5"/>
@@ -5346,7 +5394,7 @@
       <c r="M35" s="6"/>
       <c r="N35" s="5"/>
     </row>
-    <row r="36" spans="6:14">
+    <row r="36" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F36" s="1"/>
       <c r="I36" s="4"/>
       <c r="J36" s="5"/>
@@ -5355,7 +5403,7 @@
       <c r="M36" s="6"/>
       <c r="N36" s="5"/>
     </row>
-    <row r="37" spans="6:14">
+    <row r="37" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F37" s="1"/>
       <c r="I37" s="4"/>
       <c r="J37" s="5"/>
@@ -5364,7 +5412,7 @@
       <c r="M37" s="6"/>
       <c r="N37" s="5"/>
     </row>
-    <row r="38" spans="6:14">
+    <row r="38" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F38" s="1"/>
       <c r="I38" s="4"/>
       <c r="J38" s="5"/>
@@ -5373,7 +5421,7 @@
       <c r="M38" s="6"/>
       <c r="N38" s="5"/>
     </row>
-    <row r="39" spans="6:14">
+    <row r="39" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F39" s="1"/>
       <c r="I39" s="4"/>
       <c r="J39" s="5"/>
@@ -5382,7 +5430,7 @@
       <c r="M39" s="6"/>
       <c r="N39" s="5"/>
     </row>
-    <row r="40" spans="6:14">
+    <row r="40" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F40" s="1"/>
       <c r="I40" s="4"/>
       <c r="J40" s="5"/>
@@ -5391,7 +5439,7 @@
       <c r="M40" s="6"/>
       <c r="N40" s="5"/>
     </row>
-    <row r="41" spans="6:14">
+    <row r="41" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F41" s="1"/>
       <c r="I41" s="4"/>
       <c r="J41" s="5"/>
@@ -5400,7 +5448,7 @@
       <c r="M41" s="6"/>
       <c r="N41" s="5"/>
     </row>
-    <row r="42" spans="6:14">
+    <row r="42" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F42" s="1"/>
       <c r="I42" s="4"/>
       <c r="J42" s="5"/>
@@ -5409,7 +5457,7 @@
       <c r="M42" s="6"/>
       <c r="N42" s="5"/>
     </row>
-    <row r="43" spans="6:14">
+    <row r="43" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F43" s="1"/>
       <c r="I43" s="4"/>
       <c r="J43" s="5"/>
@@ -5418,7 +5466,7 @@
       <c r="M43" s="6"/>
       <c r="N43" s="5"/>
     </row>
-    <row r="44" spans="6:14">
+    <row r="44" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F44" s="1"/>
       <c r="I44" s="4"/>
       <c r="J44" s="5"/>
@@ -5427,7 +5475,7 @@
       <c r="M44" s="6"/>
       <c r="N44" s="5"/>
     </row>
-    <row r="45" spans="6:14">
+    <row r="45" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F45" s="1"/>
       <c r="I45" s="4"/>
       <c r="J45" s="5"/>
@@ -5441,6 +5489,9 @@
     <mergeCell ref="M1:M3"/>
     <mergeCell ref="D2:K2"/>
   </mergeCells>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -5450,13 +5501,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B1:N56"/>
+  <dimension ref="B1:N55"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:I18"/>
+      <selection activeCell="B5" sqref="B5:B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="8.5" customWidth="1"/>
     <col min="3" max="3" width="34.5" customWidth="1"/>
@@ -5472,12 +5523,12 @@
     <col min="14" max="14" width="8.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="41.1" customHeight="1">
+    <row r="1" spans="2:14" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M1" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:14" ht="21" customHeight="1" thickBot="1">
+    <row r="2" spans="2:14" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D2" s="13" t="s">
         <v>1</v>
       </c>
@@ -5490,10 +5541,10 @@
       <c r="K2" s="13"/>
       <c r="M2" s="11"/>
     </row>
-    <row r="3" spans="2:14" ht="16.5" thickTop="1">
+    <row r="3" spans="2:14" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="M3" s="11"/>
     </row>
-    <row r="4" spans="2:14" ht="31.5">
+    <row r="4" spans="2:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -5534,7 +5585,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:14">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2311</v>
       </c>
@@ -5575,7 +5626,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="2:14">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>2263</v>
       </c>
@@ -5616,7 +5667,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:14">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>2240</v>
       </c>
@@ -5657,7 +5708,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="2:14">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>2229</v>
       </c>
@@ -5698,7 +5749,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:14">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>2228</v>
       </c>
@@ -5739,7 +5790,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="2:14">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>2214</v>
       </c>
@@ -5780,7 +5831,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:14">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>2210</v>
       </c>
@@ -5821,7 +5872,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:14">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>2190</v>
       </c>
@@ -5862,7 +5913,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="2:14">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>2353</v>
       </c>
@@ -5903,7 +5954,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:14">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>2349</v>
       </c>
@@ -5944,7 +5995,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:14">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>2391</v>
       </c>
@@ -5985,7 +6036,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="2:14">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>2418</v>
       </c>
@@ -6026,7 +6077,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="2:14">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>2419</v>
       </c>
@@ -6067,48 +6118,16 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:14">
-      <c r="B18">
-        <v>2418</v>
-      </c>
-      <c r="C18" t="s">
-        <v>208</v>
-      </c>
-      <c r="D18" t="s">
-        <v>209</v>
-      </c>
-      <c r="E18" t="s">
-        <v>210</v>
-      </c>
-      <c r="F18" s="1">
-        <v>6</v>
-      </c>
-      <c r="G18" t="s">
-        <v>177</v>
-      </c>
-      <c r="H18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I18" s="4">
-        <v>45533</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K18" s="4">
-        <v>45534</v>
-      </c>
-      <c r="L18" s="5">
-        <v>0.375</v>
-      </c>
-      <c r="M18" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="N18" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="F18" s="1"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="5"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F19" s="1"/>
       <c r="I19" s="4"/>
       <c r="J19" s="5"/>
@@ -6117,7 +6136,7 @@
       <c r="M19" s="6"/>
       <c r="N19" s="5"/>
     </row>
-    <row r="20" spans="2:14">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F20" s="1"/>
       <c r="I20" s="4"/>
       <c r="J20" s="5"/>
@@ -6126,7 +6145,7 @@
       <c r="M20" s="6"/>
       <c r="N20" s="5"/>
     </row>
-    <row r="21" spans="2:14">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F21" s="1"/>
       <c r="I21" s="4"/>
       <c r="J21" s="5"/>
@@ -6135,7 +6154,7 @@
       <c r="M21" s="6"/>
       <c r="N21" s="5"/>
     </row>
-    <row r="22" spans="2:14">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F22" s="1"/>
       <c r="I22" s="4"/>
       <c r="J22" s="5"/>
@@ -6144,7 +6163,7 @@
       <c r="M22" s="6"/>
       <c r="N22" s="5"/>
     </row>
-    <row r="23" spans="2:14">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F23" s="1"/>
       <c r="I23" s="4"/>
       <c r="J23" s="5"/>
@@ -6153,7 +6172,7 @@
       <c r="M23" s="6"/>
       <c r="N23" s="5"/>
     </row>
-    <row r="24" spans="2:14">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F24" s="1"/>
       <c r="I24" s="4"/>
       <c r="J24" s="5"/>
@@ -6162,7 +6181,7 @@
       <c r="M24" s="6"/>
       <c r="N24" s="5"/>
     </row>
-    <row r="25" spans="2:14">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F25" s="1"/>
       <c r="I25" s="4"/>
       <c r="J25" s="5"/>
@@ -6171,7 +6190,7 @@
       <c r="M25" s="6"/>
       <c r="N25" s="5"/>
     </row>
-    <row r="26" spans="2:14">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F26" s="1"/>
       <c r="I26" s="4"/>
       <c r="J26" s="5"/>
@@ -6180,7 +6199,7 @@
       <c r="M26" s="6"/>
       <c r="N26" s="5"/>
     </row>
-    <row r="27" spans="2:14">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F27" s="1"/>
       <c r="I27" s="4"/>
       <c r="J27" s="5"/>
@@ -6189,7 +6208,7 @@
       <c r="M27" s="6"/>
       <c r="N27" s="5"/>
     </row>
-    <row r="28" spans="2:14">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F28" s="1"/>
       <c r="I28" s="4"/>
       <c r="J28" s="5"/>
@@ -6198,7 +6217,7 @@
       <c r="M28" s="6"/>
       <c r="N28" s="5"/>
     </row>
-    <row r="29" spans="2:14">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F29" s="1"/>
       <c r="I29" s="4"/>
       <c r="J29" s="5"/>
@@ -6207,7 +6226,7 @@
       <c r="M29" s="6"/>
       <c r="N29" s="5"/>
     </row>
-    <row r="30" spans="2:14">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F30" s="1"/>
       <c r="I30" s="4"/>
       <c r="J30" s="5"/>
@@ -6216,7 +6235,7 @@
       <c r="M30" s="6"/>
       <c r="N30" s="5"/>
     </row>
-    <row r="31" spans="2:14">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F31" s="1"/>
       <c r="I31" s="4"/>
       <c r="J31" s="5"/>
@@ -6225,7 +6244,8 @@
       <c r="M31" s="6"/>
       <c r="N31" s="5"/>
     </row>
-    <row r="32" spans="2:14">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="I32" s="4"/>
       <c r="J32" s="5"/>
@@ -6234,8 +6254,7 @@
       <c r="M32" s="6"/>
       <c r="N32" s="5"/>
     </row>
-    <row r="33" spans="5:14">
-      <c r="E33" s="1"/>
+    <row r="33" spans="5:14" x14ac:dyDescent="0.25">
       <c r="F33" s="1"/>
       <c r="I33" s="4"/>
       <c r="J33" s="5"/>
@@ -6244,7 +6263,8 @@
       <c r="M33" s="6"/>
       <c r="N33" s="5"/>
     </row>
-    <row r="34" spans="5:14">
+    <row r="34" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="I34" s="4"/>
       <c r="J34" s="5"/>
@@ -6253,8 +6273,7 @@
       <c r="M34" s="6"/>
       <c r="N34" s="5"/>
     </row>
-    <row r="35" spans="5:14">
-      <c r="E35" s="1"/>
+    <row r="35" spans="5:14" x14ac:dyDescent="0.25">
       <c r="F35" s="1"/>
       <c r="I35" s="4"/>
       <c r="J35" s="5"/>
@@ -6263,7 +6282,7 @@
       <c r="M35" s="6"/>
       <c r="N35" s="5"/>
     </row>
-    <row r="36" spans="5:14">
+    <row r="36" spans="5:14" x14ac:dyDescent="0.25">
       <c r="F36" s="1"/>
       <c r="I36" s="4"/>
       <c r="J36" s="5"/>
@@ -6272,7 +6291,7 @@
       <c r="M36" s="6"/>
       <c r="N36" s="5"/>
     </row>
-    <row r="37" spans="5:14">
+    <row r="37" spans="5:14" x14ac:dyDescent="0.25">
       <c r="F37" s="1"/>
       <c r="I37" s="4"/>
       <c r="J37" s="5"/>
@@ -6281,7 +6300,7 @@
       <c r="M37" s="6"/>
       <c r="N37" s="5"/>
     </row>
-    <row r="38" spans="5:14">
+    <row r="38" spans="5:14" x14ac:dyDescent="0.25">
       <c r="F38" s="1"/>
       <c r="I38" s="4"/>
       <c r="J38" s="5"/>
@@ -6290,7 +6309,7 @@
       <c r="M38" s="6"/>
       <c r="N38" s="5"/>
     </row>
-    <row r="39" spans="5:14">
+    <row r="39" spans="5:14" x14ac:dyDescent="0.25">
       <c r="F39" s="1"/>
       <c r="I39" s="4"/>
       <c r="J39" s="5"/>
@@ -6299,7 +6318,7 @@
       <c r="M39" s="6"/>
       <c r="N39" s="5"/>
     </row>
-    <row r="40" spans="5:14">
+    <row r="40" spans="5:14" x14ac:dyDescent="0.25">
       <c r="F40" s="1"/>
       <c r="I40" s="4"/>
       <c r="J40" s="5"/>
@@ -6308,7 +6327,7 @@
       <c r="M40" s="6"/>
       <c r="N40" s="5"/>
     </row>
-    <row r="41" spans="5:14">
+    <row r="41" spans="5:14" x14ac:dyDescent="0.25">
       <c r="F41" s="1"/>
       <c r="I41" s="4"/>
       <c r="J41" s="5"/>
@@ -6317,7 +6336,7 @@
       <c r="M41" s="6"/>
       <c r="N41" s="5"/>
     </row>
-    <row r="42" spans="5:14">
+    <row r="42" spans="5:14" x14ac:dyDescent="0.25">
       <c r="F42" s="1"/>
       <c r="I42" s="4"/>
       <c r="J42" s="5"/>
@@ -6326,7 +6345,7 @@
       <c r="M42" s="6"/>
       <c r="N42" s="5"/>
     </row>
-    <row r="43" spans="5:14">
+    <row r="43" spans="5:14" x14ac:dyDescent="0.25">
       <c r="F43" s="1"/>
       <c r="I43" s="4"/>
       <c r="J43" s="5"/>
@@ -6335,7 +6354,7 @@
       <c r="M43" s="6"/>
       <c r="N43" s="5"/>
     </row>
-    <row r="44" spans="5:14">
+    <row r="44" spans="5:14" x14ac:dyDescent="0.25">
       <c r="F44" s="1"/>
       <c r="I44" s="4"/>
       <c r="J44" s="5"/>
@@ -6344,7 +6363,7 @@
       <c r="M44" s="6"/>
       <c r="N44" s="5"/>
     </row>
-    <row r="45" spans="5:14">
+    <row r="45" spans="5:14" x14ac:dyDescent="0.25">
       <c r="F45" s="1"/>
       <c r="I45" s="4"/>
       <c r="J45" s="5"/>
@@ -6353,7 +6372,7 @@
       <c r="M45" s="6"/>
       <c r="N45" s="5"/>
     </row>
-    <row r="46" spans="5:14">
+    <row r="46" spans="5:14" x14ac:dyDescent="0.25">
       <c r="F46" s="1"/>
       <c r="I46" s="4"/>
       <c r="J46" s="5"/>
@@ -6362,7 +6381,7 @@
       <c r="M46" s="6"/>
       <c r="N46" s="5"/>
     </row>
-    <row r="47" spans="5:14">
+    <row r="47" spans="5:14" x14ac:dyDescent="0.25">
       <c r="F47" s="1"/>
       <c r="I47" s="4"/>
       <c r="J47" s="5"/>
@@ -6371,7 +6390,7 @@
       <c r="M47" s="6"/>
       <c r="N47" s="5"/>
     </row>
-    <row r="48" spans="5:14">
+    <row r="48" spans="5:14" x14ac:dyDescent="0.25">
       <c r="F48" s="1"/>
       <c r="I48" s="4"/>
       <c r="J48" s="5"/>
@@ -6380,7 +6399,7 @@
       <c r="M48" s="6"/>
       <c r="N48" s="5"/>
     </row>
-    <row r="49" spans="6:14">
+    <row r="49" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F49" s="1"/>
       <c r="I49" s="4"/>
       <c r="J49" s="5"/>
@@ -6389,7 +6408,7 @@
       <c r="M49" s="6"/>
       <c r="N49" s="5"/>
     </row>
-    <row r="50" spans="6:14">
+    <row r="50" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F50" s="1"/>
       <c r="I50" s="4"/>
       <c r="J50" s="5"/>
@@ -6398,7 +6417,7 @@
       <c r="M50" s="6"/>
       <c r="N50" s="5"/>
     </row>
-    <row r="51" spans="6:14">
+    <row r="51" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F51" s="1"/>
       <c r="I51" s="4"/>
       <c r="J51" s="5"/>
@@ -6407,7 +6426,7 @@
       <c r="M51" s="6"/>
       <c r="N51" s="5"/>
     </row>
-    <row r="52" spans="6:14">
+    <row r="52" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F52" s="1"/>
       <c r="I52" s="4"/>
       <c r="J52" s="5"/>
@@ -6416,7 +6435,7 @@
       <c r="M52" s="6"/>
       <c r="N52" s="5"/>
     </row>
-    <row r="53" spans="6:14">
+    <row r="53" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F53" s="1"/>
       <c r="I53" s="4"/>
       <c r="J53" s="5"/>
@@ -6425,7 +6444,7 @@
       <c r="M53" s="6"/>
       <c r="N53" s="5"/>
     </row>
-    <row r="54" spans="6:14">
+    <row r="54" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F54" s="1"/>
       <c r="I54" s="4"/>
       <c r="J54" s="5"/>
@@ -6434,7 +6453,7 @@
       <c r="M54" s="6"/>
       <c r="N54" s="5"/>
     </row>
-    <row r="55" spans="6:14">
+    <row r="55" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F55" s="1"/>
       <c r="I55" s="4"/>
       <c r="J55" s="5"/>
@@ -6443,20 +6462,14 @@
       <c r="M55" s="6"/>
       <c r="N55" s="5"/>
     </row>
-    <row r="56" spans="6:14">
-      <c r="F56" s="1"/>
-      <c r="I56" s="4"/>
-      <c r="J56" s="5"/>
-      <c r="K56" s="4"/>
-      <c r="L56" s="5"/>
-      <c r="M56" s="6"/>
-      <c r="N56" s="5"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="M1:M3"/>
     <mergeCell ref="D2:K2"/>
   </mergeCells>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -6468,11 +6481,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:N73"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="8.5" customWidth="1"/>
     <col min="3" max="3" width="34.5" customWidth="1"/>
@@ -6488,12 +6501,12 @@
     <col min="14" max="14" width="8.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="41.1" customHeight="1">
+    <row r="1" spans="2:14" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M1" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:14" ht="21" customHeight="1" thickBot="1">
+    <row r="2" spans="2:14" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D2" s="13" t="s">
         <v>1</v>
       </c>
@@ -6506,10 +6519,10 @@
       <c r="K2" s="13"/>
       <c r="M2" s="11"/>
     </row>
-    <row r="3" spans="2:14" ht="16.5" thickTop="1">
+    <row r="3" spans="2:14" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="M3" s="11"/>
     </row>
-    <row r="4" spans="2:14" ht="31.5">
+    <row r="4" spans="2:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -6550,7 +6563,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:14">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2327</v>
       </c>
@@ -6591,7 +6604,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="2:14">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>2324</v>
       </c>
@@ -6632,7 +6645,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:14">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>2323</v>
       </c>
@@ -6673,7 +6686,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="2:14">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>2312</v>
       </c>
@@ -6714,7 +6727,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:14">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>2310</v>
       </c>
@@ -6755,7 +6768,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="2:14">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>2308</v>
       </c>
@@ -6796,7 +6809,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:14">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>2302</v>
       </c>
@@ -6837,7 +6850,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:14">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>2295</v>
       </c>
@@ -6878,7 +6891,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="2:14">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>2290</v>
       </c>
@@ -6919,7 +6932,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:14">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>2276</v>
       </c>
@@ -6960,7 +6973,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:14">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>2266</v>
       </c>
@@ -7001,7 +7014,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="2:14">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>2256</v>
       </c>
@@ -7042,7 +7055,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="2:14">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>2255</v>
       </c>
@@ -7083,7 +7096,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:14">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>2251</v>
       </c>
@@ -7124,7 +7137,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:14">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>2250</v>
       </c>
@@ -7165,7 +7178,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="2:14">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>2246</v>
       </c>
@@ -7206,7 +7219,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="2:14">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>2238</v>
       </c>
@@ -7247,7 +7260,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="2:14">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>2226</v>
       </c>
@@ -7288,7 +7301,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="2:14">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>2216</v>
       </c>
@@ -7329,7 +7342,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="2:14">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>2211</v>
       </c>
@@ -7370,7 +7383,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="2:14">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>2205</v>
       </c>
@@ -7411,7 +7424,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="2:14">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>2203</v>
       </c>
@@ -7452,7 +7465,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="2:14">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>2191</v>
       </c>
@@ -7493,7 +7506,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="2:14">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="9">
         <v>2058</v>
       </c>
@@ -7534,7 +7547,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="2:14">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>1895</v>
       </c>
@@ -7575,7 +7588,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="2:14">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>2360</v>
       </c>
@@ -7616,7 +7629,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="2:14">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>2359</v>
       </c>
@@ -7657,7 +7670,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="2:14">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>2358</v>
       </c>
@@ -7698,7 +7711,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="2:14">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>2354</v>
       </c>
@@ -7739,7 +7752,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="2:14">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>2337</v>
       </c>
@@ -7780,7 +7793,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="2:14">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>2335</v>
       </c>
@@ -7821,7 +7834,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="2:14">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>2371</v>
       </c>
@@ -7862,7 +7875,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="2:14">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>2363</v>
       </c>
@@ -7903,7 +7916,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="2:14">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>2373</v>
       </c>
@@ -7944,7 +7957,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="2:14">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>2405</v>
       </c>
@@ -7985,7 +7998,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="2:14">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>2401</v>
       </c>
@@ -8026,7 +8039,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="2:14">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>2400</v>
       </c>
@@ -8067,7 +8080,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="2:14">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>2388</v>
       </c>
@@ -8108,7 +8121,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="2:14">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>2387</v>
       </c>
@@ -8149,7 +8162,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="2:14">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>2415</v>
       </c>
@@ -8190,7 +8203,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="2:14">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>2413</v>
       </c>
@@ -8231,7 +8244,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="2:14">
+    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>2410</v>
       </c>
@@ -8272,7 +8285,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="2:14">
+    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>2408</v>
       </c>
@@ -8313,7 +8326,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="2:14">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>2420</v>
       </c>
@@ -8354,7 +8367,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="6:14">
+    <row r="49" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F49" s="1"/>
       <c r="I49" s="4"/>
       <c r="J49" s="5"/>
@@ -8363,7 +8376,7 @@
       <c r="M49" s="6"/>
       <c r="N49" s="5"/>
     </row>
-    <row r="50" spans="6:14">
+    <row r="50" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F50" s="1"/>
       <c r="I50" s="4"/>
       <c r="J50" s="5"/>
@@ -8372,7 +8385,7 @@
       <c r="M50" s="6"/>
       <c r="N50" s="5"/>
     </row>
-    <row r="51" spans="6:14">
+    <row r="51" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F51" s="1"/>
       <c r="I51" s="4"/>
       <c r="J51" s="5"/>
@@ -8381,7 +8394,7 @@
       <c r="M51" s="6"/>
       <c r="N51" s="5"/>
     </row>
-    <row r="52" spans="6:14">
+    <row r="52" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F52" s="1"/>
       <c r="I52" s="4"/>
       <c r="J52" s="5"/>
@@ -8390,7 +8403,7 @@
       <c r="M52" s="6"/>
       <c r="N52" s="5"/>
     </row>
-    <row r="53" spans="6:14">
+    <row r="53" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F53" s="1"/>
       <c r="I53" s="4"/>
       <c r="J53" s="5"/>
@@ -8399,7 +8412,7 @@
       <c r="M53" s="6"/>
       <c r="N53" s="5"/>
     </row>
-    <row r="54" spans="6:14">
+    <row r="54" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F54" s="1"/>
       <c r="I54" s="4"/>
       <c r="J54" s="5"/>
@@ -8408,7 +8421,7 @@
       <c r="M54" s="6"/>
       <c r="N54" s="5"/>
     </row>
-    <row r="55" spans="6:14">
+    <row r="55" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F55" s="1"/>
       <c r="I55" s="4"/>
       <c r="J55" s="5"/>
@@ -8417,7 +8430,7 @@
       <c r="M55" s="6"/>
       <c r="N55" s="5"/>
     </row>
-    <row r="56" spans="6:14">
+    <row r="56" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F56" s="1"/>
       <c r="I56" s="4"/>
       <c r="J56" s="5"/>
@@ -8426,7 +8439,7 @@
       <c r="M56" s="6"/>
       <c r="N56" s="5"/>
     </row>
-    <row r="57" spans="6:14">
+    <row r="57" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F57" s="1"/>
       <c r="I57" s="4"/>
       <c r="J57" s="5"/>
@@ -8435,7 +8448,7 @@
       <c r="M57" s="6"/>
       <c r="N57" s="5"/>
     </row>
-    <row r="58" spans="6:14">
+    <row r="58" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F58" s="1"/>
       <c r="I58" s="4"/>
       <c r="J58" s="5"/>
@@ -8444,7 +8457,7 @@
       <c r="M58" s="6"/>
       <c r="N58" s="5"/>
     </row>
-    <row r="59" spans="6:14">
+    <row r="59" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F59" s="1"/>
       <c r="I59" s="4"/>
       <c r="J59" s="5"/>
@@ -8453,7 +8466,7 @@
       <c r="M59" s="6"/>
       <c r="N59" s="5"/>
     </row>
-    <row r="60" spans="6:14">
+    <row r="60" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F60" s="1"/>
       <c r="I60" s="4"/>
       <c r="J60" s="5"/>
@@ -8462,7 +8475,7 @@
       <c r="M60" s="6"/>
       <c r="N60" s="5"/>
     </row>
-    <row r="61" spans="6:14">
+    <row r="61" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F61" s="1"/>
       <c r="I61" s="4"/>
       <c r="J61" s="5"/>
@@ -8471,7 +8484,7 @@
       <c r="M61" s="6"/>
       <c r="N61" s="5"/>
     </row>
-    <row r="62" spans="6:14">
+    <row r="62" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F62" s="1"/>
       <c r="I62" s="4"/>
       <c r="J62" s="5"/>
@@ -8480,7 +8493,7 @@
       <c r="M62" s="6"/>
       <c r="N62" s="5"/>
     </row>
-    <row r="63" spans="6:14">
+    <row r="63" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F63" s="1"/>
       <c r="I63" s="4"/>
       <c r="J63" s="5"/>
@@ -8489,7 +8502,7 @@
       <c r="M63" s="6"/>
       <c r="N63" s="5"/>
     </row>
-    <row r="64" spans="6:14">
+    <row r="64" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F64" s="1"/>
       <c r="I64" s="4"/>
       <c r="J64" s="5"/>
@@ -8498,7 +8511,7 @@
       <c r="M64" s="6"/>
       <c r="N64" s="5"/>
     </row>
-    <row r="65" spans="5:14">
+    <row r="65" spans="5:14" x14ac:dyDescent="0.25">
       <c r="F65" s="1"/>
       <c r="I65" s="4"/>
       <c r="J65" s="5"/>
@@ -8507,7 +8520,7 @@
       <c r="M65" s="6"/>
       <c r="N65" s="5"/>
     </row>
-    <row r="66" spans="5:14">
+    <row r="66" spans="5:14" x14ac:dyDescent="0.25">
       <c r="F66" s="1"/>
       <c r="I66" s="4"/>
       <c r="J66" s="5"/>
@@ -8516,7 +8529,7 @@
       <c r="M66" s="6"/>
       <c r="N66" s="5"/>
     </row>
-    <row r="67" spans="5:14">
+    <row r="67" spans="5:14" x14ac:dyDescent="0.25">
       <c r="F67" s="1"/>
       <c r="I67" s="4"/>
       <c r="J67" s="5"/>
@@ -8525,7 +8538,7 @@
       <c r="M67" s="6"/>
       <c r="N67" s="5"/>
     </row>
-    <row r="68" spans="5:14">
+    <row r="68" spans="5:14" x14ac:dyDescent="0.25">
       <c r="F68" s="1"/>
       <c r="I68" s="4"/>
       <c r="J68" s="5"/>
@@ -8534,7 +8547,7 @@
       <c r="M68" s="6"/>
       <c r="N68" s="5"/>
     </row>
-    <row r="69" spans="5:14">
+    <row r="69" spans="5:14" x14ac:dyDescent="0.25">
       <c r="F69" s="1"/>
       <c r="I69" s="4"/>
       <c r="J69" s="5"/>
@@ -8543,7 +8556,7 @@
       <c r="M69" s="6"/>
       <c r="N69" s="5"/>
     </row>
-    <row r="70" spans="5:14">
+    <row r="70" spans="5:14" x14ac:dyDescent="0.25">
       <c r="F70" s="1"/>
       <c r="I70" s="4"/>
       <c r="J70" s="5"/>
@@ -8552,7 +8565,7 @@
       <c r="M70" s="6"/>
       <c r="N70" s="5"/>
     </row>
-    <row r="71" spans="5:14">
+    <row r="71" spans="5:14" x14ac:dyDescent="0.25">
       <c r="F71" s="1"/>
       <c r="I71" s="4"/>
       <c r="J71" s="5"/>
@@ -8561,7 +8574,7 @@
       <c r="M71" s="6"/>
       <c r="N71" s="5"/>
     </row>
-    <row r="72" spans="5:14">
+    <row r="72" spans="5:14" x14ac:dyDescent="0.25">
       <c r="F72" s="1"/>
       <c r="I72" s="4"/>
       <c r="J72" s="5"/>
@@ -8570,7 +8583,7 @@
       <c r="M72" s="6"/>
       <c r="N72" s="5"/>
     </row>
-    <row r="73" spans="5:14">
+    <row r="73" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="I73" s="4"/>
@@ -8585,6 +8598,9 @@
     <mergeCell ref="D2:K2"/>
     <mergeCell ref="M1:M3"/>
   </mergeCells>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
@@ -8597,11 +8613,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="8.5" customWidth="1"/>
     <col min="3" max="3" width="34.5" customWidth="1"/>
@@ -8617,12 +8633,12 @@
     <col min="14" max="14" width="8.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="41.1" customHeight="1">
+    <row r="1" spans="2:14" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M1" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:14" ht="21" customHeight="1" thickBot="1">
+    <row r="2" spans="2:14" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D2" s="13" t="s">
         <v>1</v>
       </c>
@@ -8635,10 +8651,10 @@
       <c r="K2" s="13"/>
       <c r="M2" s="11"/>
     </row>
-    <row r="3" spans="2:14" ht="16.5" thickTop="1">
+    <row r="3" spans="2:14" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="M3" s="11"/>
     </row>
-    <row r="4" spans="2:14" ht="31.5">
+    <row r="4" spans="2:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -8679,7 +8695,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:14">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2303</v>
       </c>
@@ -8720,7 +8736,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="2:14">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>2301</v>
       </c>
@@ -8761,7 +8777,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:14">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>2300</v>
       </c>
@@ -8802,7 +8818,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="2:14">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>2281</v>
       </c>
@@ -8843,7 +8859,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:14">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>2275</v>
       </c>
@@ -8884,7 +8900,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="2:14">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>2273</v>
       </c>
@@ -8925,7 +8941,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:14">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>2244</v>
       </c>
@@ -8966,7 +8982,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:14">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>2236</v>
       </c>
@@ -9007,7 +9023,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="2:14">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>2235</v>
       </c>
@@ -9048,7 +9064,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:14">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>2218</v>
       </c>
@@ -9089,7 +9105,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:14">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>2196</v>
       </c>
@@ -9130,7 +9146,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="2:14">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>1714</v>
       </c>
@@ -9171,7 +9187,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="2:14">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>1897</v>
       </c>
@@ -9212,7 +9228,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:14">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>2346</v>
       </c>
@@ -9253,7 +9269,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:14">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>2370</v>
       </c>
@@ -9294,7 +9310,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="2:14">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>2365</v>
       </c>
@@ -9335,7 +9351,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="2:14">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>2404</v>
       </c>
@@ -9376,7 +9392,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="2:14">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>2384</v>
       </c>
@@ -9417,7 +9433,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="2:14">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>2380</v>
       </c>
@@ -9458,7 +9474,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="2:14">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>2414</v>
       </c>
@@ -9499,7 +9515,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="2:14">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F25" s="1"/>
       <c r="I25" s="4"/>
       <c r="J25" s="5"/>
@@ -9508,7 +9524,7 @@
       <c r="M25" s="6"/>
       <c r="N25" s="5"/>
     </row>
-    <row r="26" spans="2:14">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F26" s="1"/>
       <c r="I26" s="4"/>
       <c r="J26" s="5"/>
@@ -9517,7 +9533,7 @@
       <c r="M26" s="6"/>
       <c r="N26" s="5"/>
     </row>
-    <row r="27" spans="2:14">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F27" s="1"/>
       <c r="I27" s="4"/>
       <c r="J27" s="5"/>
@@ -9526,7 +9542,7 @@
       <c r="M27" s="6"/>
       <c r="N27" s="5"/>
     </row>
-    <row r="28" spans="2:14">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F28" s="1"/>
       <c r="I28" s="4"/>
       <c r="J28" s="5"/>
@@ -9535,7 +9551,7 @@
       <c r="M28" s="6"/>
       <c r="N28" s="5"/>
     </row>
-    <row r="29" spans="2:14">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F29" s="1"/>
       <c r="I29" s="4"/>
       <c r="J29" s="5"/>
@@ -9544,7 +9560,7 @@
       <c r="M29" s="6"/>
       <c r="N29" s="5"/>
     </row>
-    <row r="30" spans="2:14">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F30" s="1"/>
       <c r="I30" s="4"/>
       <c r="J30" s="5"/>
@@ -9553,7 +9569,7 @@
       <c r="M30" s="6"/>
       <c r="N30" s="5"/>
     </row>
-    <row r="31" spans="2:14">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="I31" s="4"/>
@@ -9563,7 +9579,7 @@
       <c r="M31" s="6"/>
       <c r="N31" s="5"/>
     </row>
-    <row r="32" spans="2:14">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F32" s="1"/>
       <c r="I32" s="4"/>
       <c r="J32" s="5"/>
@@ -9572,7 +9588,7 @@
       <c r="M32" s="6"/>
       <c r="N32" s="5"/>
     </row>
-    <row r="33" spans="6:14">
+    <row r="33" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F33" s="1"/>
       <c r="I33" s="4"/>
       <c r="J33" s="5"/>
@@ -9581,7 +9597,7 @@
       <c r="M33" s="6"/>
       <c r="N33" s="5"/>
     </row>
-    <row r="34" spans="6:14">
+    <row r="34" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F34" s="1"/>
       <c r="I34" s="4"/>
       <c r="J34" s="5"/>
@@ -9590,7 +9606,7 @@
       <c r="M34" s="6"/>
       <c r="N34" s="5"/>
     </row>
-    <row r="35" spans="6:14">
+    <row r="35" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F35" s="1"/>
       <c r="I35" s="4"/>
       <c r="J35" s="5"/>
@@ -9599,7 +9615,7 @@
       <c r="M35" s="6"/>
       <c r="N35" s="5"/>
     </row>
-    <row r="36" spans="6:14">
+    <row r="36" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F36" s="1"/>
       <c r="I36" s="4"/>
       <c r="J36" s="5"/>
@@ -9608,7 +9624,7 @@
       <c r="M36" s="6"/>
       <c r="N36" s="5"/>
     </row>
-    <row r="37" spans="6:14">
+    <row r="37" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F37" s="1"/>
       <c r="I37" s="4"/>
       <c r="J37" s="5"/>
@@ -9617,7 +9633,7 @@
       <c r="M37" s="6"/>
       <c r="N37" s="5"/>
     </row>
-    <row r="38" spans="6:14">
+    <row r="38" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F38" s="1"/>
       <c r="I38" s="4"/>
       <c r="J38" s="5"/>
@@ -9626,7 +9642,7 @@
       <c r="M38" s="6"/>
       <c r="N38" s="5"/>
     </row>
-    <row r="39" spans="6:14">
+    <row r="39" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F39" s="1"/>
       <c r="I39" s="4"/>
       <c r="J39" s="5"/>
@@ -9635,7 +9651,7 @@
       <c r="M39" s="6"/>
       <c r="N39" s="5"/>
     </row>
-    <row r="40" spans="6:14">
+    <row r="40" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F40" s="1"/>
       <c r="I40" s="4"/>
       <c r="J40" s="5"/>
@@ -9644,7 +9660,7 @@
       <c r="M40" s="6"/>
       <c r="N40" s="5"/>
     </row>
-    <row r="41" spans="6:14">
+    <row r="41" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F41" s="1"/>
       <c r="I41" s="4"/>
       <c r="J41" s="5"/>
@@ -9653,7 +9669,7 @@
       <c r="M41" s="6"/>
       <c r="N41" s="5"/>
     </row>
-    <row r="42" spans="6:14">
+    <row r="42" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F42" s="1"/>
       <c r="I42" s="4"/>
       <c r="J42" s="5"/>
@@ -9662,7 +9678,7 @@
       <c r="M42" s="6"/>
       <c r="N42" s="5"/>
     </row>
-    <row r="43" spans="6:14">
+    <row r="43" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F43" s="1"/>
       <c r="I43" s="4"/>
       <c r="J43" s="5"/>
@@ -9671,7 +9687,7 @@
       <c r="M43" s="6"/>
       <c r="N43" s="5"/>
     </row>
-    <row r="44" spans="6:14">
+    <row r="44" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F44" s="1"/>
       <c r="I44" s="4"/>
       <c r="J44" s="5"/>
@@ -9680,7 +9696,7 @@
       <c r="M44" s="6"/>
       <c r="N44" s="5"/>
     </row>
-    <row r="45" spans="6:14">
+    <row r="45" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F45" s="1"/>
       <c r="I45" s="4"/>
       <c r="J45" s="5"/>
@@ -9689,7 +9705,7 @@
       <c r="M45" s="6"/>
       <c r="N45" s="5"/>
     </row>
-    <row r="46" spans="6:14">
+    <row r="46" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F46" s="1"/>
       <c r="I46" s="4"/>
       <c r="J46" s="5"/>
@@ -9698,7 +9714,7 @@
       <c r="M46" s="6"/>
       <c r="N46" s="5"/>
     </row>
-    <row r="47" spans="6:14">
+    <row r="47" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F47" s="1"/>
       <c r="I47" s="4"/>
       <c r="J47" s="5"/>
@@ -9707,7 +9723,7 @@
       <c r="M47" s="6"/>
       <c r="N47" s="5"/>
     </row>
-    <row r="48" spans="6:14">
+    <row r="48" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F48" s="1"/>
       <c r="I48" s="4"/>
       <c r="J48" s="5"/>
@@ -9716,7 +9732,7 @@
       <c r="M48" s="6"/>
       <c r="N48" s="5"/>
     </row>
-    <row r="49" spans="6:14">
+    <row r="49" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F49" s="1"/>
       <c r="I49" s="4"/>
       <c r="J49" s="5"/>
@@ -9725,7 +9741,7 @@
       <c r="M49" s="6"/>
       <c r="N49" s="5"/>
     </row>
-    <row r="50" spans="6:14">
+    <row r="50" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F50" s="1"/>
       <c r="I50" s="4"/>
       <c r="J50" s="5"/>
@@ -9734,7 +9750,7 @@
       <c r="M50" s="6"/>
       <c r="N50" s="5"/>
     </row>
-    <row r="51" spans="6:14">
+    <row r="51" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F51" s="1"/>
       <c r="I51" s="4"/>
       <c r="J51" s="5"/>

</xml_diff>